<commit_message>
Implemented csv download and fixed some bugs in dynamic UI rendering
</commit_message>
<xml_diff>
--- a/ODMAP_spreadsheet.xlsx
+++ b/ODMAP_spreadsheet.xlsx
@@ -1083,6 +1083,126 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1122,139 +1242,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1542,7 +1542,7 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
@@ -1558,72 +1558,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
       <c r="I1" s="4" t="s">
         <v>31</v>
       </c>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="60"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
       <c r="I2" s="4" t="s">
         <v>32</v>
       </c>
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
       <c r="I3" s="4" t="s">
         <v>105</v>
       </c>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="60"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
       <c r="I4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="60"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="66"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="53"/>
       <c r="I5" s="4" t="s">
         <v>106</v>
       </c>
@@ -1631,85 +1631,85 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="30" t="s">
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="30" t="s">
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="29"/>
-      <c r="I7" s="31"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="71"/>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="36" t="s">
+      <c r="A8" s="36"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="40" t="s">
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
       <c r="I8" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
       <c r="I9" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
       <c r="I10" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="48"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="76"/>
       <c r="I11" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="41"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="32"/>
       <c r="G12" s="12"/>
       <c r="H12" s="14"/>
       <c r="I12" s="13" t="s">
@@ -1717,163 +1717,163 @@
       </c>
     </row>
     <row r="13" spans="1:10" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="41" t="s">
+      <c r="A13" s="36"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="45"/>
-      <c r="H13" s="42"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="43"/>
       <c r="I13" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
       <c r="I14" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
       <c r="F15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
       <c r="I15" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="41" t="s">
+      <c r="A16" s="36"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
       <c r="I16" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
       <c r="I17" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
       <c r="I18" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
       <c r="I19" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
       <c r="I20" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
       <c r="I21" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="41" t="s">
+      <c r="A22" s="36"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
       <c r="I22" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
       <c r="I23" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="41" t="s">
+      <c r="A24" s="36"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="32" t="s">
         <v>11</v>
       </c>
       <c r="G24" s="15"/>
@@ -1883,247 +1883,247 @@
       </c>
     </row>
     <row r="25" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
       <c r="I25" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
       <c r="I26" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
       <c r="F27" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
       <c r="I27" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
       <c r="F28" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
       <c r="I28" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
       <c r="I29" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
       <c r="F30" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
       <c r="I30" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="34"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
       <c r="F31" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
       <c r="I31" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="51"/>
-      <c r="C32" s="52" t="s">
+      <c r="A32" s="34"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="40" t="s">
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
       <c r="I32" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
       <c r="I33" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
       <c r="I34" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
       <c r="I35" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
       <c r="I36" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
       <c r="I37" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="46"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
       <c r="I38" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
       <c r="I39" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="41" t="s">
+      <c r="A40" s="36"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
       <c r="I40" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="45"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
       <c r="I41" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="55"/>
-      <c r="F42" s="41" t="s">
+      <c r="A42" s="36"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="32" t="s">
         <v>18</v>
       </c>
       <c r="G42" s="12"/>
@@ -2133,12 +2133,12 @@
       </c>
     </row>
     <row r="43" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="55"/>
-      <c r="F43" s="41"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="32"/>
       <c r="G43" s="12"/>
       <c r="H43" s="14"/>
       <c r="I43" s="5" t="s">
@@ -2146,324 +2146,324 @@
       </c>
     </row>
     <row r="44" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
-      <c r="B44" s="33"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="41"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
       <c r="I44" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
-      <c r="B45" s="33"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="41" t="s">
+      <c r="A45" s="36"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="44"/>
       <c r="I45" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="32"/>
-      <c r="B46" s="33"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="46"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="55"/>
+      <c r="H46" s="55"/>
       <c r="I46" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="32"/>
-      <c r="B47" s="33"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
+      <c r="A47" s="36"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
       <c r="I47" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="3" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
-      <c r="B48" s="33"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="46"/>
-      <c r="H48" s="46"/>
+      <c r="A48" s="36"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="55"/>
       <c r="I48" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
-      <c r="B49" s="33"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="46"/>
-      <c r="H49" s="46"/>
+      <c r="A49" s="36"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="55"/>
+      <c r="H49" s="55"/>
       <c r="I49" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="32"/>
-      <c r="B50" s="33"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="47"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="41" t="s">
+      <c r="A50" s="36"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G50" s="47"/>
-      <c r="H50" s="47"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
       <c r="I50" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
-      <c r="B51" s="33"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
+      <c r="A51" s="36"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
       <c r="I51" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="32"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="41"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
+      <c r="A52" s="36"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="46"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="46"/>
+      <c r="H52" s="46"/>
       <c r="I52" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="32"/>
-      <c r="B53" s="33"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="46"/>
-      <c r="H53" s="46"/>
+      <c r="A53" s="36"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="55"/>
+      <c r="H53" s="55"/>
       <c r="I53" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="34"/>
-      <c r="B54" s="35"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="59"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
+      <c r="A54" s="38"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="47"/>
+      <c r="E54" s="47"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="47"/>
+      <c r="H54" s="47"/>
       <c r="I54" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="50"/>
-      <c r="B55" s="51"/>
-      <c r="C55" s="52" t="s">
+      <c r="A55" s="34"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="D55" s="42"/>
-      <c r="E55" s="42"/>
+      <c r="D55" s="43"/>
+      <c r="E55" s="43"/>
       <c r="F55" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G55" s="42"/>
-      <c r="H55" s="42"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="43"/>
       <c r="I55" s="7" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="32"/>
-      <c r="B56" s="33"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="41"/>
-      <c r="E56" s="41"/>
+      <c r="A56" s="36"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
       <c r="F56" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G56" s="41"/>
-      <c r="H56" s="41"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
       <c r="I56" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="32"/>
-      <c r="B57" s="33"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
-      <c r="F57" s="41" t="s">
+      <c r="A57" s="36"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="G57" s="45"/>
-      <c r="H57" s="45"/>
+      <c r="G57" s="44"/>
+      <c r="H57" s="44"/>
       <c r="I57" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="32"/>
-      <c r="B58" s="33"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="41"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
+      <c r="A58" s="36"/>
+      <c r="B58" s="37"/>
+      <c r="C58" s="41"/>
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="44"/>
+      <c r="H58" s="44"/>
       <c r="I58" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="32"/>
-      <c r="B59" s="33"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="41"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="45"/>
+      <c r="A59" s="36"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="32"/>
+      <c r="G59" s="44"/>
+      <c r="H59" s="44"/>
       <c r="I59" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
-      <c r="B60" s="33"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="45"/>
-      <c r="E60" s="45"/>
-      <c r="F60" s="41"/>
-      <c r="G60" s="47"/>
-      <c r="H60" s="47"/>
+      <c r="A60" s="36"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="41"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="46"/>
+      <c r="H60" s="46"/>
       <c r="I60" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="3" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="32"/>
-      <c r="B61" s="33"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="22"/>
-      <c r="E61" s="23"/>
-      <c r="F61" s="19" t="s">
+      <c r="A61" s="36"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="62"/>
+      <c r="E61" s="63"/>
+      <c r="F61" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="G61" s="41"/>
-      <c r="H61" s="41"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="32"/>
       <c r="I61" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="32"/>
-      <c r="B62" s="33"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="41"/>
-      <c r="H62" s="41"/>
+      <c r="A62" s="36"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="64"/>
+      <c r="E62" s="65"/>
+      <c r="F62" s="60"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="32"/>
       <c r="I62" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="32"/>
-      <c r="B63" s="33"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="41"/>
-      <c r="H63" s="41"/>
+      <c r="A63" s="36"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="41"/>
+      <c r="D63" s="66"/>
+      <c r="E63" s="67"/>
+      <c r="F63" s="61"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
       <c r="I63" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="32"/>
-      <c r="B64" s="33"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="45"/>
-      <c r="E64" s="45"/>
-      <c r="F64" s="41" t="s">
+      <c r="A64" s="36"/>
+      <c r="B64" s="37"/>
+      <c r="C64" s="41"/>
+      <c r="D64" s="44"/>
+      <c r="E64" s="44"/>
+      <c r="F64" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="G64" s="45"/>
-      <c r="H64" s="45"/>
+      <c r="G64" s="44"/>
+      <c r="H64" s="44"/>
       <c r="I64" s="5" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="32"/>
-      <c r="B65" s="33"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="45"/>
-      <c r="E65" s="45"/>
-      <c r="F65" s="41"/>
-      <c r="G65" s="41"/>
-      <c r="H65" s="41"/>
+      <c r="A65" s="36"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="41"/>
+      <c r="D65" s="44"/>
+      <c r="E65" s="44"/>
+      <c r="F65" s="32"/>
+      <c r="G65" s="32"/>
+      <c r="H65" s="32"/>
       <c r="I65" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="32"/>
-      <c r="B66" s="33"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="45"/>
-      <c r="E66" s="45"/>
-      <c r="F66" s="41"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="41"/>
+      <c r="A66" s="36"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="41"/>
+      <c r="D66" s="44"/>
+      <c r="E66" s="44"/>
+      <c r="F66" s="32"/>
+      <c r="G66" s="32"/>
+      <c r="H66" s="32"/>
       <c r="I66" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="34"/>
-      <c r="B67" s="35"/>
-      <c r="C67" s="37"/>
+      <c r="A67" s="38"/>
+      <c r="B67" s="39"/>
+      <c r="C67" s="42"/>
       <c r="D67" s="16"/>
       <c r="E67" s="17"/>
       <c r="F67" s="10" t="s">
@@ -2476,29 +2476,29 @@
       </c>
     </row>
     <row r="68" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="50"/>
-      <c r="B68" s="51"/>
-      <c r="C68" s="52" t="s">
+      <c r="A68" s="34"/>
+      <c r="B68" s="35"/>
+      <c r="C68" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="D68" s="42"/>
-      <c r="E68" s="42"/>
-      <c r="F68" s="40" t="s">
+      <c r="D68" s="43"/>
+      <c r="E68" s="43"/>
+      <c r="F68" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="G68" s="42"/>
-      <c r="H68" s="42"/>
+      <c r="G68" s="43"/>
+      <c r="H68" s="43"/>
       <c r="I68" s="7" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="32"/>
-      <c r="B69" s="33"/>
-      <c r="C69" s="36"/>
-      <c r="D69" s="45"/>
-      <c r="E69" s="45"/>
-      <c r="F69" s="41"/>
+      <c r="A69" s="36"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="44"/>
+      <c r="E69" s="44"/>
+      <c r="F69" s="32"/>
       <c r="G69" s="12"/>
       <c r="H69" s="14"/>
       <c r="I69" s="5" t="s">
@@ -2506,12 +2506,12 @@
       </c>
     </row>
     <row r="70" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="32"/>
-      <c r="B70" s="33"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="45"/>
-      <c r="E70" s="45"/>
-      <c r="F70" s="41"/>
+      <c r="A70" s="36"/>
+      <c r="B70" s="37"/>
+      <c r="C70" s="41"/>
+      <c r="D70" s="44"/>
+      <c r="E70" s="44"/>
+      <c r="F70" s="32"/>
       <c r="G70" s="12"/>
       <c r="H70" s="14"/>
       <c r="I70" s="5" t="s">
@@ -2519,11 +2519,11 @@
       </c>
     </row>
     <row r="71" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="32"/>
-      <c r="B71" s="33"/>
-      <c r="C71" s="36"/>
-      <c r="D71" s="45"/>
-      <c r="E71" s="45"/>
+      <c r="A71" s="36"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="41"/>
+      <c r="D71" s="44"/>
+      <c r="E71" s="44"/>
       <c r="F71" s="9" t="s">
         <v>28</v>
       </c>
@@ -2534,11 +2534,11 @@
       </c>
     </row>
     <row r="72" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="34"/>
-      <c r="B72" s="35"/>
-      <c r="C72" s="37"/>
-      <c r="D72" s="49"/>
-      <c r="E72" s="49"/>
+      <c r="A72" s="38"/>
+      <c r="B72" s="39"/>
+      <c r="C72" s="42"/>
+      <c r="D72" s="45"/>
+      <c r="E72" s="45"/>
       <c r="F72" s="10" t="s">
         <v>29</v>
       </c>
@@ -2549,55 +2549,55 @@
       </c>
     </row>
     <row r="73" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="67"/>
-      <c r="B73" s="69"/>
-      <c r="C73" s="71" t="s">
+      <c r="A73" s="19"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D73" s="73"/>
-      <c r="E73" s="75"/>
-      <c r="F73" s="40" t="s">
+      <c r="D73" s="25"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G73" s="40"/>
-      <c r="H73" s="40"/>
+      <c r="G73" s="31"/>
+      <c r="H73" s="31"/>
       <c r="I73" s="7" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="67"/>
-      <c r="B74" s="69"/>
-      <c r="C74" s="71"/>
-      <c r="D74" s="54"/>
-      <c r="E74" s="55"/>
-      <c r="F74" s="41"/>
-      <c r="G74" s="41"/>
-      <c r="H74" s="41"/>
+      <c r="A74" s="19"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="32"/>
+      <c r="G74" s="32"/>
+      <c r="H74" s="32"/>
       <c r="I74" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="67"/>
-      <c r="B75" s="69"/>
-      <c r="C75" s="71"/>
-      <c r="D75" s="54"/>
-      <c r="E75" s="55"/>
-      <c r="F75" s="41"/>
-      <c r="G75" s="41"/>
-      <c r="H75" s="41"/>
+      <c r="A75" s="19"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="26"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="32"/>
+      <c r="G75" s="32"/>
+      <c r="H75" s="32"/>
       <c r="I75" s="5" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="67"/>
-      <c r="B76" s="69"/>
-      <c r="C76" s="71"/>
-      <c r="D76" s="54"/>
-      <c r="E76" s="55"/>
-      <c r="F76" s="41"/>
+      <c r="A76" s="19"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="23"/>
+      <c r="D76" s="26"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="32"/>
       <c r="G76" s="12"/>
       <c r="H76" s="14"/>
       <c r="I76" s="5" t="s">
@@ -2605,27 +2605,27 @@
       </c>
     </row>
     <row r="77" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="67"/>
-      <c r="B77" s="69"/>
-      <c r="C77" s="71"/>
-      <c r="D77" s="54"/>
-      <c r="E77" s="55"/>
-      <c r="F77" s="41"/>
-      <c r="G77" s="47"/>
-      <c r="H77" s="47"/>
+      <c r="A77" s="19"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="26"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="32"/>
+      <c r="G77" s="46"/>
+      <c r="H77" s="46"/>
       <c r="I77" s="5" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="78" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="68"/>
-      <c r="B78" s="70"/>
-      <c r="C78" s="72"/>
-      <c r="D78" s="74"/>
-      <c r="E78" s="76"/>
-      <c r="F78" s="59"/>
-      <c r="G78" s="58"/>
-      <c r="H78" s="58"/>
+      <c r="A78" s="20"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="27"/>
+      <c r="E78" s="30"/>
+      <c r="F78" s="33"/>
+      <c r="G78" s="47"/>
+      <c r="H78" s="47"/>
       <c r="I78" s="6" t="s">
         <v>99</v>
       </c>
@@ -2635,30 +2635,76 @@
     </row>
   </sheetData>
   <mergeCells count="123">
-    <mergeCell ref="A73:A78"/>
-    <mergeCell ref="B73:B78"/>
-    <mergeCell ref="C73:C78"/>
-    <mergeCell ref="D73:D78"/>
-    <mergeCell ref="E73:E78"/>
-    <mergeCell ref="F73:F78"/>
-    <mergeCell ref="A68:B72"/>
-    <mergeCell ref="C68:C72"/>
-    <mergeCell ref="D68:E70"/>
-    <mergeCell ref="F68:F70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="F61:F63"/>
+    <mergeCell ref="D61:E63"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="A8:B31"/>
+    <mergeCell ref="C8:C31"/>
+    <mergeCell ref="D8:E12"/>
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="D16:E21"/>
+    <mergeCell ref="F16:F21"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="D22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="D24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A32:B54"/>
+    <mergeCell ref="C32:C54"/>
+    <mergeCell ref="D32:E39"/>
+    <mergeCell ref="F32:F39"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="D40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="D45:E49"/>
+    <mergeCell ref="F45:F49"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:H31"/>
     <mergeCell ref="A1:F5"/>
     <mergeCell ref="A55:B67"/>
     <mergeCell ref="C55:C67"/>
@@ -2683,81 +2729,35 @@
     <mergeCell ref="D50:E54"/>
     <mergeCell ref="F50:F54"/>
     <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="G51:H51"/>
     <mergeCell ref="G52:H52"/>
     <mergeCell ref="G53:H53"/>
     <mergeCell ref="G54:H54"/>
-    <mergeCell ref="D45:E49"/>
-    <mergeCell ref="F45:F49"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A32:B54"/>
-    <mergeCell ref="C32:C54"/>
-    <mergeCell ref="D32:E39"/>
-    <mergeCell ref="F32:F39"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="D40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="D22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="D24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="F61:F63"/>
-    <mergeCell ref="D61:E63"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:B31"/>
-    <mergeCell ref="C8:C31"/>
-    <mergeCell ref="D8:E12"/>
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="D16:E21"/>
-    <mergeCell ref="F16:F21"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="D13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A73:A78"/>
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="C73:C78"/>
+    <mergeCell ref="D73:D78"/>
+    <mergeCell ref="E73:E78"/>
+    <mergeCell ref="F73:F78"/>
+    <mergeCell ref="A68:B72"/>
+    <mergeCell ref="C68:C72"/>
+    <mergeCell ref="D68:E70"/>
+    <mergeCell ref="F68:F70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="67" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Damaris: minimal reordering of ODMAP table
</commit_message>
<xml_diff>
--- a/ODMAP_spreadsheet.xlsx
+++ b/ODMAP_spreadsheet.xlsx
@@ -389,9 +389,6 @@
     <t>o  ecological inference/explanation</t>
   </si>
   <si>
-    <t>o  mapping</t>
-  </si>
-  <si>
     <t>o  forecast/transfer</t>
   </si>
   <si>
@@ -475,6 +472,9 @@
   </si>
   <si>
     <t>Variable importance</t>
+  </si>
+  <si>
+    <t>o  mapping/interpolation</t>
   </si>
 </sst>
 </file>
@@ -583,7 +583,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -620,6 +620,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -770,7 +776,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -782,8 +788,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -814,32 +830,74 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -859,22 +917,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -895,51 +947,52 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="21">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1210,7 +1263,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1223,8 +1276,8 @@
   </sheetPr>
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1239,157 +1292,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
       <c r="I1" s="10" t="s">
         <v>22</v>
       </c>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="15">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="15">
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="15">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="15">
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" ht="15">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="10" t="s">
-        <v>108</v>
-      </c>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="15">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="40"/>
       <c r="I5" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="7" spans="1:10" customFormat="1" ht="15">
+      <c r="A7" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="7" spans="1:10" customFormat="1" ht="15">
-      <c r="A7" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30" t="s">
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:10" customFormat="1" ht="15">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="17" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="12" t="s">
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
       <c r="I8" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:10" customFormat="1" ht="15">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
       <c r="I9" s="6" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:10" customFormat="1" ht="15">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
       <c r="I10" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" customFormat="1" ht="15">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:10" customFormat="1" ht="15">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
     <row r="12" spans="1:10" customFormat="1" ht="15">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="12"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="7"/>
       <c r="H12" s="8"/>
       <c r="I12" s="5" t="s">
@@ -1397,163 +1450,163 @@
       </c>
     </row>
     <row r="13" spans="1:10" customFormat="1" ht="15">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="12" t="s">
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
       <c r="I13" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:10" customFormat="1" ht="15">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
       <c r="I14" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:10" customFormat="1" ht="15">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
       <c r="F15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
       <c r="I15" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:10" customFormat="1" ht="15">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="12" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
       <c r="I16" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:9" customFormat="1" ht="15">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
       <c r="I17" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:9" customFormat="1" ht="15">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
       <c r="I18" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:9" customFormat="1" ht="15">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
       <c r="I19" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:9" customFormat="1" ht="15">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
       <c r="I20" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:9" customFormat="1" ht="15">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
       <c r="I21" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:9" customFormat="1" ht="15">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="12" t="s">
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
       <c r="I22" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:9" customFormat="1" ht="15">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
       <c r="I23" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:9" customFormat="1" ht="15">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="12" t="s">
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="27" t="s">
         <v>5</v>
       </c>
       <c r="G24" s="9"/>
@@ -1563,245 +1616,245 @@
       </c>
     </row>
     <row r="25" spans="1:9" customFormat="1" ht="15">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
       <c r="I25" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:9" customFormat="1" ht="15">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
       <c r="I26" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:9" customFormat="1" ht="15">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
       <c r="F27" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
       <c r="I27" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:9" customFormat="1" ht="15">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
       <c r="F28" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
       <c r="I28" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:9" customFormat="1" ht="15">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
       <c r="I29" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:9" customFormat="1" ht="15">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
       <c r="F30" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
       <c r="I30" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:9" customFormat="1" ht="15">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
       <c r="F31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
       <c r="I31" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:9" customFormat="1" ht="15">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="17" t="s">
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="12" t="s">
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
       <c r="I32" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:9" customFormat="1" ht="15">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
       <c r="I33" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:9" customFormat="1" ht="30">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
       <c r="I34" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:9" customFormat="1" ht="15">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
       <c r="I35" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:9" customFormat="1" ht="15">
-      <c r="A36" s="20"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
       <c r="I36" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:9" customFormat="1" ht="15">
-      <c r="A37" s="20"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
       <c r="I37" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:9" customFormat="1" ht="30">
-      <c r="A38" s="20"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
       <c r="I38" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:9" customFormat="1" ht="30">
-      <c r="A39" s="20"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
       <c r="I39" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:9" customFormat="1" ht="30">
-      <c r="A40" s="20"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
       <c r="I40" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:9" customFormat="1" ht="30">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
       <c r="I41" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:9" customFormat="1" ht="15">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="12" t="s">
+      <c r="A42" s="25"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="27" t="s">
         <v>10</v>
       </c>
       <c r="G42" s="7"/>
@@ -1811,12 +1864,12 @@
       </c>
     </row>
     <row r="43" spans="1:9" customFormat="1" ht="30">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="12"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="27"/>
       <c r="G43" s="7"/>
       <c r="H43" s="8"/>
       <c r="I43" s="5" t="s">
@@ -1824,352 +1877,352 @@
       </c>
     </row>
     <row r="44" spans="1:9" customFormat="1" ht="15">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
       <c r="I44" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:9" customFormat="1" ht="15">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="12" t="s">
+      <c r="A45" s="25"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
       <c r="I45" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:9" customFormat="1" ht="15">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
       <c r="I46" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:9" customFormat="1" ht="15">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28"/>
       <c r="I47" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:9" customFormat="1" ht="45">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="28"/>
+      <c r="A48" s="25"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
       <c r="I48" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:9" customFormat="1" ht="30">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="28"/>
+      <c r="A49" s="25"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
       <c r="I49" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:9" customFormat="1" ht="15">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="12" t="s">
+      <c r="A50" s="25"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
       <c r="I50" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:9" customFormat="1" ht="15">
-      <c r="A51" s="20"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
+      <c r="A51" s="25"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="33"/>
+      <c r="H51" s="33"/>
       <c r="I51" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:9" customFormat="1" ht="15">
-      <c r="A52" s="20"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
+      <c r="A52" s="25"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="33"/>
       <c r="I52" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:9" customFormat="1" ht="15">
-      <c r="A53" s="20"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="28"/>
-      <c r="H53" s="28"/>
+      <c r="A53" s="25"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32"/>
       <c r="I53" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:9" customFormat="1" ht="30">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
+      <c r="A54" s="25"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
       <c r="I54" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:9" customFormat="1" ht="30">
-      <c r="A55" s="20"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="17" t="s">
+      <c r="A55" s="25"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
       <c r="F55" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G55" s="27"/>
-      <c r="H55" s="27"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="28"/>
       <c r="I55" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:9" customFormat="1" ht="30">
-      <c r="A56" s="20"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
+      <c r="A56" s="25"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
       <c r="F56" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
       <c r="I56" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:9" customFormat="1" ht="30">
-      <c r="A57" s="20"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="12" t="s">
+      <c r="A57" s="25"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="G57" s="27"/>
-      <c r="H57" s="27"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="28"/>
       <c r="I57" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:9" customFormat="1" ht="15">
-      <c r="A58" s="20"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="27"/>
-      <c r="H58" s="27"/>
+      <c r="A58" s="25"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="28"/>
+      <c r="H58" s="28"/>
       <c r="I58" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:9" customFormat="1" ht="15">
-      <c r="A59" s="20"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
+      <c r="A59" s="25"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="33"/>
       <c r="I59" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:9" customFormat="1" ht="15">
-      <c r="A60" s="20"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="39" t="s">
+      <c r="A60" s="25"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="45"/>
+      <c r="E60" s="46"/>
+      <c r="F60" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G60" s="9"/>
       <c r="H60" s="8"/>
       <c r="I60" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" customFormat="1" ht="15">
+      <c r="A61" s="25"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="48"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" customFormat="1" ht="15">
+      <c r="A62" s="25"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="49"/>
+      <c r="E62" s="50"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="61" spans="1:9" customFormat="1" ht="15">
-      <c r="A61" s="20"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="35"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="40"/>
-      <c r="G61" s="42"/>
-      <c r="H61" s="43"/>
-      <c r="I61" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" customFormat="1" ht="15">
-      <c r="A62" s="20"/>
-      <c r="B62" s="20"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="38"/>
-      <c r="F62" s="41"/>
-      <c r="G62" s="42"/>
-      <c r="H62" s="43"/>
-      <c r="I62" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
     <row r="63" spans="1:9" customFormat="1" ht="45" customHeight="1">
-      <c r="A63" s="20"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="44"/>
-      <c r="E63" s="45"/>
-      <c r="F63" s="39" t="s">
+      <c r="A63" s="25"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="27"/>
       <c r="I63" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:9" customFormat="1" ht="15">
-      <c r="A64" s="20"/>
-      <c r="B64" s="20"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="46"/>
-      <c r="E64" s="47"/>
-      <c r="F64" s="40"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
+      <c r="A64" s="25"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="27"/>
+      <c r="H64" s="27"/>
       <c r="I64" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:9" customFormat="1" ht="15">
-      <c r="A65" s="20"/>
-      <c r="B65" s="20"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="48"/>
-      <c r="E65" s="49"/>
-      <c r="F65" s="41"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
+      <c r="A65" s="25"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="27"/>
+      <c r="H65" s="27"/>
       <c r="I65" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:9" customFormat="1" ht="15">
-      <c r="A66" s="20"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="12" t="s">
+      <c r="A66" s="25"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="31"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="G66" s="27"/>
-      <c r="H66" s="27"/>
+      <c r="G66" s="28"/>
+      <c r="H66" s="28"/>
       <c r="I66" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:9" customFormat="1" ht="15">
-      <c r="A67" s="20"/>
-      <c r="B67" s="20"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="12"/>
+      <c r="A67" s="25"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="26"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="27"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="27"/>
       <c r="I67" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:9" customFormat="1" ht="15">
-      <c r="A68" s="20"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="12"/>
+      <c r="A68" s="25"/>
+      <c r="B68" s="25"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="31"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="27"/>
+      <c r="H68" s="27"/>
       <c r="I68" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:9" customFormat="1" ht="15">
-      <c r="A69" s="20"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="17"/>
+      <c r="A69" s="25"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="26"/>
       <c r="D69" s="3"/>
       <c r="E69" s="4"/>
       <c r="F69" s="5" t="s">
@@ -2181,73 +2234,73 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:9" customFormat="1" ht="15">
-      <c r="A70" s="20"/>
-      <c r="B70" s="20"/>
-      <c r="C70" s="17" t="s">
+    <row r="70" spans="1:9" customFormat="1" ht="16" customHeight="1">
+      <c r="A70" s="51"/>
+      <c r="B70" s="52"/>
+      <c r="C70" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="12" t="s">
+      <c r="D70" s="57"/>
+      <c r="E70" s="58"/>
+      <c r="F70" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G70" s="9"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" customFormat="1" ht="15" customHeight="1">
+      <c r="A71" s="53"/>
+      <c r="B71" s="54"/>
+      <c r="C71" s="56"/>
+      <c r="D71" s="45"/>
+      <c r="E71" s="46"/>
+      <c r="F71" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="G70" s="27"/>
-      <c r="H70" s="27"/>
-      <c r="I70" s="5" t="s">
+      <c r="G71" s="28"/>
+      <c r="H71" s="28"/>
+      <c r="I71" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:9" customFormat="1" ht="15">
-      <c r="A71" s="20"/>
-      <c r="B71" s="20"/>
-      <c r="C71" s="17"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="13"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
     <row r="72" spans="1:9" customFormat="1" ht="15">
-      <c r="A72" s="20"/>
-      <c r="B72" s="20"/>
-      <c r="C72" s="17"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="12"/>
+      <c r="A72" s="53"/>
+      <c r="B72" s="54"/>
+      <c r="C72" s="56"/>
+      <c r="D72" s="47"/>
+      <c r="E72" s="48"/>
+      <c r="F72" s="27"/>
       <c r="G72" s="7"/>
       <c r="H72" s="8"/>
       <c r="I72" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:9" customFormat="1" ht="15">
-      <c r="A73" s="20"/>
-      <c r="B73" s="20"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G73" s="9"/>
+      <c r="A73" s="53"/>
+      <c r="B73" s="54"/>
+      <c r="C73" s="56"/>
+      <c r="D73" s="49"/>
+      <c r="E73" s="50"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="7"/>
       <c r="H73" s="8"/>
       <c r="I73" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:9" customFormat="1" ht="15">
-      <c r="A74" s="15"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="17" t="s">
+      <c r="A74" s="41"/>
+      <c r="B74" s="42"/>
+      <c r="C74" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="D74" s="18"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="12" t="s">
+      <c r="D74" s="43"/>
+      <c r="E74" s="44"/>
+      <c r="F74" s="27" t="s">
         <v>84</v>
       </c>
       <c r="G74" s="7"/>
@@ -2257,102 +2310,207 @@
       </c>
     </row>
     <row r="75" spans="1:9" customFormat="1" ht="15">
-      <c r="A75" s="15"/>
-      <c r="B75" s="16"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="12"/>
+      <c r="A75" s="41"/>
+      <c r="B75" s="42"/>
+      <c r="C75" s="26"/>
+      <c r="D75" s="43"/>
+      <c r="E75" s="44"/>
+      <c r="F75" s="27"/>
+      <c r="G75" s="27"/>
+      <c r="H75" s="27"/>
       <c r="I75" s="5" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:9" customFormat="1" ht="15">
-      <c r="A76" s="15"/>
-      <c r="B76" s="16"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="19"/>
-      <c r="F76" s="12" t="s">
+      <c r="A76" s="41"/>
+      <c r="B76" s="42"/>
+      <c r="C76" s="26"/>
+      <c r="D76" s="43"/>
+      <c r="E76" s="44"/>
+      <c r="F76" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="G76" s="12"/>
-      <c r="H76" s="12"/>
+      <c r="G76" s="27"/>
+      <c r="H76" s="27"/>
       <c r="I76" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:9" customFormat="1" ht="15">
-      <c r="A77" s="15"/>
-      <c r="B77" s="16"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="18"/>
-      <c r="E77" s="19"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
+      <c r="A77" s="41"/>
+      <c r="B77" s="42"/>
+      <c r="C77" s="26"/>
+      <c r="D77" s="43"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="27"/>
+      <c r="G77" s="27"/>
+      <c r="H77" s="27"/>
       <c r="I77" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:9" customFormat="1" ht="15">
-      <c r="A78" s="15"/>
-      <c r="B78" s="16"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="19"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
+      <c r="A78" s="41"/>
+      <c r="B78" s="42"/>
+      <c r="C78" s="26"/>
+      <c r="D78" s="43"/>
+      <c r="E78" s="44"/>
+      <c r="F78" s="27"/>
+      <c r="G78" s="27"/>
+      <c r="H78" s="27"/>
       <c r="I78" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:9" customFormat="1" ht="15">
-      <c r="A79" s="15"/>
-      <c r="B79" s="16"/>
-      <c r="C79" s="17"/>
-      <c r="D79" s="18"/>
-      <c r="E79" s="19"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
+      <c r="A79" s="41"/>
+      <c r="B79" s="42"/>
+      <c r="C79" s="26"/>
+      <c r="D79" s="43"/>
+      <c r="E79" s="44"/>
+      <c r="F79" s="27"/>
+      <c r="G79" s="33"/>
+      <c r="H79" s="33"/>
       <c r="I79" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:9" customFormat="1" ht="15">
-      <c r="A80" s="15"/>
-      <c r="B80" s="16"/>
-      <c r="C80" s="17"/>
-      <c r="D80" s="18"/>
-      <c r="E80" s="19"/>
-      <c r="F80" s="12"/>
-      <c r="G80" s="11"/>
-      <c r="H80" s="11"/>
+      <c r="A80" s="41"/>
+      <c r="B80" s="42"/>
+      <c r="C80" s="26"/>
+      <c r="D80" s="43"/>
+      <c r="E80" s="44"/>
+      <c r="F80" s="27"/>
+      <c r="G80" s="33"/>
+      <c r="H80" s="33"/>
       <c r="I80" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:9" customFormat="1" ht="15">
-      <c r="A81" s="15"/>
-      <c r="B81" s="16"/>
-      <c r="C81" s="17"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="14"/>
+      <c r="A81" s="41"/>
+      <c r="B81" s="42"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="17"/>
       <c r="F81" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
+      <c r="G81" s="27"/>
+      <c r="H81" s="27"/>
       <c r="I81" s="5" t="s">
         <v>91</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="129">
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="D45:E49"/>
+    <mergeCell ref="F45:F49"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="D60:E62"/>
+    <mergeCell ref="A70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E73"/>
+    <mergeCell ref="D32:E41"/>
+    <mergeCell ref="F32:F41"/>
+    <mergeCell ref="D57:E59"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="D50:E54"/>
+    <mergeCell ref="F50:F54"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="F71:F73"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="A74:A81"/>
+    <mergeCell ref="B74:B81"/>
+    <mergeCell ref="C74:C81"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="D76:D80"/>
+    <mergeCell ref="E76:E80"/>
+    <mergeCell ref="F76:F80"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="A1:F5"/>
+    <mergeCell ref="A55:B69"/>
+    <mergeCell ref="C55:C69"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="D66:E68"/>
+    <mergeCell ref="F66:F68"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="A32:B54"/>
+    <mergeCell ref="C32:C54"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="D22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="D24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="G28:H28"/>
     <mergeCell ref="F60:F62"/>
     <mergeCell ref="G61:H61"/>
     <mergeCell ref="G62:H62"/>
@@ -2377,111 +2535,6 @@
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="D13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="D22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="D24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A1:F5"/>
-    <mergeCell ref="A55:B69"/>
-    <mergeCell ref="C55:C69"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="D66:E68"/>
-    <mergeCell ref="F66:F68"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="A32:B54"/>
-    <mergeCell ref="C32:C54"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="A70:B73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="D70:E72"/>
-    <mergeCell ref="F70:F72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="A74:A81"/>
-    <mergeCell ref="B74:B81"/>
-    <mergeCell ref="C74:C81"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="D76:D80"/>
-    <mergeCell ref="E76:E80"/>
-    <mergeCell ref="F76:F80"/>
-    <mergeCell ref="G80:H80"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="D32:E41"/>
-    <mergeCell ref="F32:F41"/>
-    <mergeCell ref="D57:E59"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="D50:E54"/>
-    <mergeCell ref="F50:F54"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="D45:E49"/>
-    <mergeCell ref="F45:F49"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="D60:E62"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.71" right="0.71" top="0.75000000000000011" bottom="0.75000000000000011" header="0.31" footer="0.31"/>

</xml_diff>